<commit_message>
Add an update to new component
</commit_message>
<xml_diff>
--- a/PracticeAngular/SomeNotesOnAngular.xlsx
+++ b/PracticeAngular/SomeNotesOnAngular.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/datngo/Documents/projects/angularp/bringItToWorkBench/MyWorkspace/PracticeAngular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86772A9-FAF9-6648-98B2-41DCB4F84103}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD544A72-D545-AC4A-B841-87D5F4D3E5FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{0F100960-46C4-7B4F-A190-71D233F84722}"/>
+    <workbookView xWindow="37640" yWindow="-24840" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{0F100960-46C4-7B4F-A190-71D233F84722}"/>
   </bookViews>
   <sheets>
     <sheet name="Directive" sheetId="1" r:id="rId1"/>
+    <sheet name="UsingBootstrap" sheetId="2" r:id="rId2"/>
+    <sheet name="NewComponent" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,6 +24,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Add this</t>
+  </si>
+  <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>1. Generate</t>
+  </si>
+  <si>
+    <t>2. Declare</t>
+  </si>
+  <si>
+    <t>3. Use</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,6 +353,704 @@
         </a:prstGeom>
         <a:noFill/>
         <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBC7E48E-BD99-054D-8939-06A14C945F1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="368300" y="368300"/>
+          <a:ext cx="2552700" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>--install Bootstrap v3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>  $ npm install --save bootstrap@3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{544E626E-3DE0-1746-B602-1ED2AB73D586}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3213100" y="355600"/>
+          <a:ext cx="2552700" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>edit: angular.json</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61B8908A-DE0D-2849-BA37-C0A9AB7D7419}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6286500" y="254000"/>
+          <a:ext cx="5854700" cy="2108200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17DD0DC8-7065-0348-8CB4-61E1718472D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11468100" y="1739900"/>
+          <a:ext cx="1612900" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>317499</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>249890</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A792731B-E420-5741-84D6-3B5FA65F5280}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6349999" y="3048000"/>
+          <a:ext cx="6282391" cy="3073400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E61CC2D-759D-184D-A1D2-4AC6DA811414}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10515600" y="5384800"/>
+          <a:ext cx="2374900" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{356D833D-2EAE-3B4B-B9AC-97F4B354D788}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="431800" y="381000"/>
+          <a:ext cx="3022600" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>  $ ng generate component servers </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>  OR </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>  $ ng g c servers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C13BD03-D255-104B-9C7A-A487F1A5A58B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3848100" y="355600"/>
+          <a:ext cx="6718300" cy="5943600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4CF0B68-9B70-C048-845E-6360731F4650}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4546600" y="2044700"/>
+          <a:ext cx="5943600" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33128984-6B4C-5A4B-B018-092CF60DE19A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4876800" y="3365500"/>
+          <a:ext cx="2247900" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF4A08C7-0906-4644-9471-C8B14C27D645}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11112500" y="609600"/>
+          <a:ext cx="3962400" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC859668-E4B0-134E-AA1B-C9F016E017E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11341100" y="1473200"/>
+          <a:ext cx="4051300" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
           <a:solidFill>
             <a:srgbClr val="FF0000"/>
           </a:solidFill>
@@ -664,7 +1385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB83D6F-9532-7A44-B867-31763F07C422}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AE17" sqref="AE17"/>
     </sheetView>
   </sheetViews>
@@ -673,4 +1394,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199AD069-6237-7C4A-99C8-85DEA761C6F8}">
+  <dimension ref="AP9:AP27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AP28" sqref="AP28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="9" spans="42:42" x14ac:dyDescent="0.2">
+      <c r="AP9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="42:42" x14ac:dyDescent="0.2">
+      <c r="AP27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156FC777-D7ED-B142-9306-0C3917927B60}">
+  <dimension ref="B1:AJ2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ3" sqref="AJ3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="4.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AJ2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add demo code for angular 4 forms of binding
</commit_message>
<xml_diff>
--- a/PracticeAngular/SomeNotesOnAngular.xlsx
+++ b/PracticeAngular/SomeNotesOnAngular.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/datngo/Documents/projects/angularp/bringItToWorkBench/MyWorkspace/PracticeAngular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C12B67-E759-6D4D-B09F-134D4EA0A798}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DB3879-4D9E-B44F-8D46-4AB5B58BFBD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41980" yWindow="-27440" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{0F100960-46C4-7B4F-A190-71D233F84722}"/>
+    <workbookView xWindow="45120" yWindow="-21680" windowWidth="28040" windowHeight="17440" xr2:uid="{0F100960-46C4-7B4F-A190-71D233F84722}"/>
   </bookViews>
   <sheets>
-    <sheet name="Directive" sheetId="1" r:id="rId1"/>
+    <sheet name="Directives" sheetId="1" r:id="rId1"/>
     <sheet name="UsingBootstrap" sheetId="2" r:id="rId2"/>
     <sheet name="NewComponent" sheetId="3" r:id="rId3"/>
     <sheet name="Selector" sheetId="4" r:id="rId4"/>
     <sheet name="SampleAppMockup" sheetId="5" r:id="rId5"/>
     <sheet name="AngularBootstrap" sheetId="6" r:id="rId6"/>
     <sheet name="DataBinding" sheetId="7" r:id="rId7"/>
+    <sheet name="EventBinding" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Add this</t>
   </si>
@@ -107,12 +108,54 @@
   <si>
     <t>và cũng không thể kết hợp 2 cách này lại với nhau</t>
   </si>
+  <si>
+    <t>$ sign event will simply be the data emitted with that event</t>
+  </si>
+  <si>
+    <t>Two way data-binding</t>
+  </si>
+  <si>
+    <t>We use the syntax as : [(ngModel)]="&lt;… something here ...&gt;"</t>
+  </si>
+  <si>
+    <t>NOTE: to be able to use ngModel, we have to add import for FormsModule (from @angular/forms) into imports[] wihin AppModule</t>
+  </si>
+  <si>
+    <t>This setup will trigger input event, and upte value of "serverName" at the same tie.</t>
+  </si>
+  <si>
+    <t>Refer to sheet "EventBinding"</t>
+  </si>
+  <si>
+    <t>This is a 2 way bindin, so that, if we change vaue of "serverName" it will also update value displayed at input element</t>
+  </si>
+  <si>
+    <t>Directives are instructionin the DOM</t>
+  </si>
+  <si>
+    <t>Componets are kinds of such instruction sin the DOM.</t>
+  </si>
+  <si>
+    <t>They are directives with a template</t>
+  </si>
+  <si>
+    <t>There are also directives without templates</t>
+  </si>
+  <si>
+    <t>E.g as below image</t>
+  </si>
+  <si>
+    <t>This is a directive, with attribute selector</t>
+  </si>
+  <si>
+    <t>Here , we. Define directive with directive decorator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,6 +166,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -149,10 +200,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,6 +508,287 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{696E6683-2F35-7F49-BC9B-62FE6D9BE36A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="635000" y="5892800"/>
+          <a:ext cx="7404100" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EED8A371-E617-4649-8AEC-C23ED4C64EC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3492500" y="6705600"/>
+          <a:ext cx="4991100" cy="2209800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{620F87AB-AC4F-0E4C-AAD3-42B2A88012B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5245100" y="7010400"/>
+          <a:ext cx="2349500" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Oval 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C71D4714-77BE-8D4C-8BE3-39B3F216771D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2781300" y="6210300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Elbow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53A5576B-9C38-6A47-8DAB-FB61655FAE42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="0"/>
+          <a:endCxn id="10" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="4314825" y="4905375"/>
+          <a:ext cx="723900" cy="3486150"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2785,6 +3118,415 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="13" name="Group 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90FA07E2-3669-044E-870A-BA69A25CEF7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="546100" y="12344400"/>
+          <a:ext cx="4064000" cy="1752600"/>
+          <a:chOff x="546100" y="12344400"/>
+          <a:chExt cx="4064000" cy="1752600"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="12" name="Picture 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAE0E2AB-AB49-7D49-98A9-4D8F3C1E7AD7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="685800" y="12344400"/>
+            <a:ext cx="3924300" cy="1752600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{005AE993-27E9-5647-B0E6-C38BEBF9EBD0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="546100" y="13322300"/>
+            <a:ext cx="1397000" cy="254000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Group 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A5E90BA-4BB3-154D-9320-18C33A187EDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="635000" y="609600"/>
+          <a:ext cx="5130800" cy="3175000"/>
+          <a:chOff x="635000" y="609600"/>
+          <a:chExt cx="5130800" cy="3175000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="2" name="Picture 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6505CF0-7F1E-5F47-B429-0C9DF74283F0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="635000" y="609600"/>
+            <a:ext cx="5130800" cy="3175000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{562CD4AF-8996-3A44-B6BA-99FF57119016}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3302000" y="1549400"/>
+            <a:ext cx="139700" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FEF4572-43AF-3641-85CD-F5834C60964A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1689100" y="4127500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Elbow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4407A4AF-2E4E-3A49-AF22-FBE89D746583}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="5" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1431925" y="2263775"/>
+          <a:ext cx="2197100" cy="1682750"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 48266"/>
+            <a:gd name="adj2" fmla="val 113585"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C97133F-A89B-3540-95E8-BDBCB08D382C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="635000" y="4470400"/>
+          <a:ext cx="6197600" cy="787400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3087,14 +3829,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB83D6F-9532-7A44-B867-31763F07C422}">
-  <dimension ref="A1"/>
+  <dimension ref="A23:AB36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE17" sqref="AE17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="AB37" sqref="AB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="AB36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3182,7 +3960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0D9EF1-ECBF-A74E-9234-0311E4C269D2}">
   <dimension ref="A2:C70"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -3261,7 +4039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3654BAC2-51D7-E44E-9E77-B954E47649E5}">
   <dimension ref="B2:AP39"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
@@ -3300,10 +4078,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0B5FE5-D25D-D643-ADEB-55FFEFE27EE7}">
-  <dimension ref="A2:W38"/>
+  <dimension ref="A2:W73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="W39" sqref="W39"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="R64" sqref="R64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3336,6 +4114,57 @@
         <v>24</v>
       </c>
     </row>
+    <row r="57" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3552393-B0D4-1148-9E49-3ABD83A665D3}">
+  <dimension ref="G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
provide more  samples on directives
</commit_message>
<xml_diff>
--- a/PracticeAngular/SomeNotesOnAngular.xlsx
+++ b/PracticeAngular/SomeNotesOnAngular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/datngo/Documents/projects/angularp/bringItToWorkBench/MyWorkspace/PracticeAngular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DB3879-4D9E-B44F-8D46-4AB5B58BFBD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077F9169-5779-424E-9FA1-1D2AA3823473}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45120" yWindow="-21680" windowWidth="28040" windowHeight="17440" xr2:uid="{0F100960-46C4-7B4F-A190-71D233F84722}"/>
+    <workbookView xWindow="45140" yWindow="-21680" windowWidth="28040" windowHeight="17440" xr2:uid="{0F100960-46C4-7B4F-A190-71D233F84722}"/>
   </bookViews>
   <sheets>
     <sheet name="Directives" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Add this</t>
   </si>
@@ -150,12 +150,108 @@
   <si>
     <t>Here , we. Define directive with directive decorator</t>
   </si>
+  <si>
+    <t>Structural directive</t>
+  </si>
+  <si>
+    <t>ngIF</t>
+  </si>
+  <si>
+    <t>Because it change the DOM (i.e add or not to add some element(s)) based on a conition</t>
+  </si>
+  <si>
+    <t>The value should be a boolean variable, or a function returns boolean</t>
+  </si>
+  <si>
+    <t>A local reference</t>
+  </si>
+  <si>
+    <t>can be considered as a "marker"</t>
+  </si>
+  <si>
+    <t>Directive "ng-template"</t>
+  </si>
+  <si>
+    <t>used to mark places in the DOM</t>
+  </si>
+  <si>
+    <t>Attribute directives</t>
+  </si>
+  <si>
+    <t>it does not add or remove elements. it only changes the element it was placed on</t>
+  </si>
+  <si>
+    <t>NOTE: remember that square bracket is not a part of ngStyle directive</t>
+  </si>
+  <si>
+    <t>The second part is a Boolean condition, so that it determine whether this css Class to be added or not</t>
+  </si>
+  <si>
+    <t>The first part is the name of the Css Class</t>
+  </si>
+  <si>
+    <t>ngFor directive</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An example with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>ngStyle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> directive. This directive require some pre-condition to do something. That's why we will use property binding on this</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Another attribute directive is "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>ngClass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Note: we must have * as a prefix for ngFor</t>
+  </si>
+  <si>
+    <t>We can track for index of each iteration by this method</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +274,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -226,23 +328,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>54454</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A932198E-C7D6-D944-B18C-D8E1A25A8DF1}"/>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{156FE4CE-2FCB-4745-B885-638B8244DBD1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -258,8 +360,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="304799" y="190500"/>
-          <a:ext cx="6417155" cy="3962400"/>
+          <a:off x="635000" y="12598400"/>
+          <a:ext cx="4279900" cy="990600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -270,23 +372,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>54454</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC6F3F8-CD31-1D46-9D3E-05741F695F03}"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A932198E-C7D6-D944-B18C-D8E1A25A8DF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -296,6 +398,50 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="304799" y="190500"/>
+          <a:ext cx="6417155" cy="3962400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC6F3F8-CD31-1D46-9D3E-05741F695F03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -537,7 +683,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -581,7 +727,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -763,6 +909,1446 @@
         <a:xfrm rot="16200000" flipV="1">
           <a:off x="4314825" y="4905375"/>
           <a:ext cx="723900" cy="3486150"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C53AA91-0969-B445-A254-7947D2790A8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="635000" y="9956800"/>
+          <a:ext cx="7721600" cy="292100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF9F5E59-D9FD-BA45-ADA7-1231697C47D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="927100" y="9931400"/>
+          <a:ext cx="2032000" cy="431800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Elbow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A1E230E-7223-C643-8A75-D6D7355104BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1936750" y="10369550"/>
+          <a:ext cx="406400" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA489438-1301-CE43-BBDA-D85A531E05D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2908300" y="12547600"/>
+          <a:ext cx="1397000" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Oval 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BABCDE20-7220-5942-A44C-A672B0D0054C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4064000" y="12776200"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>231682</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>104682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66582</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>117382</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Elbow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F02DFF27-ABE1-204D-A45F-6C441E679396}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="22" idx="5"/>
+          <a:endCxn id="25" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3374932" y="12303032"/>
+          <a:ext cx="215900" cy="1422400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 216220"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Oval 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DD81664-EFDA-AC43-868F-D68774EB2CD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2641600" y="12992100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C15D7D5-93DD-6A42-A31C-97387CDA5E04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="15036800"/>
+          <a:ext cx="6350000" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rectangle 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{550B17F8-75AD-704F-8BAF-DC7C9B10AA01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1231900" y="15011400"/>
+          <a:ext cx="927100" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C05E7C18-D467-F74C-ABCB-08AB43DAD3F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="16129000"/>
+          <a:ext cx="6350000" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A3ACDE0-F833-374A-8ABE-FD959D5C7823}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="17614900"/>
+          <a:ext cx="2425700" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Rectangle 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F92F649-BA71-CD45-A2FE-3B47EDE58695}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="16344900"/>
+          <a:ext cx="901700" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectangle 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1174032-9D6C-3E4E-825A-F716D8F6971D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2857500" y="16344900"/>
+          <a:ext cx="2451100" cy="825500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Oval 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9BF554B-3A6A-BD4B-B729-B1040BEB2826}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1981200" y="16929100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Elbow Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59340C3F-374E-084C-A977-B30FBD3B3C9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="34" idx="6"/>
+          <a:endCxn id="37" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="914400" y="17005300"/>
+          <a:ext cx="1219200" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector5">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -18750"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+            <a:gd name="adj3" fmla="val 118750"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Oval 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECEFB660-489F-4246-8F62-1CBB2E5808C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="17691100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Oval 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D15D1957-CF6F-6D4F-A36D-C575C20104FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2997200" y="16954500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>136618</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>73118</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Elbow Connector 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FECB6B59-39F4-0B4C-BCFD-2DB2949A1251}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="39" idx="4"/>
+          <a:endCxn id="43" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3448050" y="16732250"/>
+          <a:ext cx="441418" cy="1190718"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Oval 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3642EF24-E010-1F4A-95CF-E236BC327D8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4241800" y="17526000"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EAAC67C-3958-4F42-BC20-3E771CE21979}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="965200" y="14198600"/>
+          <a:ext cx="5321300" cy="292100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A163489-C0DF-7341-ABB1-5312E58BC9C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="14884400"/>
+          <a:ext cx="5321300" cy="977900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Rectangle 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A00E056B-5A3F-4142-906E-194471ED298A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4178300" y="14782800"/>
+          <a:ext cx="1485900" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Oval 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A90CF53-F5E3-C74B-B804-BF0AC8A86FE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7086600" y="14732000"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>244382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>123918</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Elbow Connector 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C1A2282-451E-134C-B881-D65B10EF772A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="47" idx="3"/>
+          <a:endCxn id="48" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5664200" y="14862082"/>
+          <a:ext cx="1444718" cy="98518"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -3829,47 +5415,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB83D6F-9532-7A44-B867-31763F07C422}">
-  <dimension ref="A23:AB36"/>
+  <dimension ref="A23:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="AB37" sqref="AB37"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="X73" sqref="X73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="B26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="B29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28">
       <c r="C33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="3:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28">
       <c r="AB36" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28">
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="G54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7">
+      <c r="C57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="B60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="C61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" ht="21">
+      <c r="B69" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" ht="21">
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="1:24" ht="21">
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:24" ht="21">
+      <c r="B72" s="3"/>
+      <c r="C72" t="s">
+        <v>55</v>
+      </c>
+      <c r="X72" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" ht="21">
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:24" ht="21">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:24" ht="21">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:24" ht="21">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:24">
+      <c r="A77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24">
+      <c r="B78" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" ht="21">
+      <c r="B80" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="81" spans="2:15">
+      <c r="C81" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="87" spans="2:15" ht="21">
+      <c r="B87" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="2:15">
+      <c r="O95" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="5:5">
+      <c r="E101" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3886,14 +5582,14 @@
       <selection activeCell="AP28" sqref="AP28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="9" spans="42:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="42:42">
       <c r="AP9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="42:42" x14ac:dyDescent="0.2">
+    <row r="27" spans="42:42">
       <c r="AP27" t="s">
         <v>1</v>
       </c>
@@ -3912,12 +5608,12 @@
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="12" max="12" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:36">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3925,27 +5621,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:36">
       <c r="AJ2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="B35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="C36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -3964,52 +5660,52 @@
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3">
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="B49" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="C50" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="B53" s="2"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2">
       <c r="B70" t="s">
         <v>19</v>
       </c>
@@ -4028,7 +5724,7 @@
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4043,29 +5739,29 @@
       <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3">
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="41:42" x14ac:dyDescent="0.2">
+    <row r="38" spans="41:42">
       <c r="AO38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="41:42" x14ac:dyDescent="0.2">
+    <row r="39" spans="41:42">
       <c r="AP39" t="s">
         <v>9</v>
       </c>
@@ -4084,62 +5780,62 @@
       <selection activeCell="R64" sqref="R64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2">
       <c r="B2" s="2"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="22:23">
       <c r="V34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="22:23">
       <c r="W35" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="22:23">
       <c r="V37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="22:23">
       <c r="W38" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="21">
       <c r="A57" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2">
       <c r="B59" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2">
       <c r="B60" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:5">
       <c r="D71" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:5">
       <c r="E72" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:5">
       <c r="D73" t="s">
         <v>31</v>
       </c>
@@ -4158,9 +5854,9 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7">
       <c r="G21" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
add some notes while learning angular security
</commit_message>
<xml_diff>
--- a/PracticeAngular/SomeNotesOnAngular.xlsx
+++ b/PracticeAngular/SomeNotesOnAngular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/datngo/Documents/projects/angularp/bringItToWorkBench/MyWorkspace/PracticeAngular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077F9169-5779-424E-9FA1-1D2AA3823473}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42190DE-AFF2-B54E-AE0A-6EFAD6E49941}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45140" yWindow="-21680" windowWidth="28040" windowHeight="17440" xr2:uid="{0F100960-46C4-7B4F-A190-71D233F84722}"/>
+    <workbookView xWindow="40600" yWindow="-28280" windowWidth="26640" windowHeight="19280" activeTab="8" xr2:uid="{0F100960-46C4-7B4F-A190-71D233F84722}"/>
   </bookViews>
   <sheets>
     <sheet name="Directives" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="AngularBootstrap" sheetId="6" r:id="rId6"/>
     <sheet name="DataBinding" sheetId="7" r:id="rId7"/>
     <sheet name="EventBinding" sheetId="8" r:id="rId8"/>
+    <sheet name="Observable" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -5417,7 +5418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB83D6F-9532-7A44-B867-31763F07C422}">
   <dimension ref="A23:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="X73" sqref="X73"/>
     </sheetView>
   </sheetViews>
@@ -5865,4 +5866,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDAD810-8EEC-2644-A6F9-5A62FBB97B72}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AK21" sqref="AK21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>